<commit_message>
added matrices file with common matrix generators
</commit_message>
<xml_diff>
--- a/lab6_cpp/Results.xlsx
+++ b/lab6_cpp/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tempRepo\sem5\DS\DS_labs3\lab6_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF951F1-B2C7-4F35-97C5-028820E60FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DC0E17-3A52-480A-9C41-6C198B0B522D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C4ADCE2E-1671-4732-8DDF-8B5F524DD51A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Matrix Size</t>
   </si>
@@ -52,6 +52,51 @@
   </si>
   <si>
     <t>Fox</t>
+  </si>
+  <si>
+    <t>0.0071</t>
+  </si>
+  <si>
+    <t>0.1292</t>
+  </si>
+  <si>
+    <t>1.2083</t>
+  </si>
+  <si>
+    <t>25.1591</t>
+  </si>
+  <si>
+    <t>242.1411</t>
+  </si>
+  <si>
+    <t>50.1231</t>
+  </si>
+  <si>
+    <t>4.8309</t>
+  </si>
+  <si>
+    <t>2.4463</t>
+  </si>
+  <si>
+    <t>10.2846</t>
+  </si>
+  <si>
+    <t>0.2472</t>
+  </si>
+  <si>
+    <t>4.8870</t>
+  </si>
+  <si>
+    <t>0.0017</t>
+  </si>
+  <si>
+    <t>4.2527</t>
+  </si>
+  <si>
+    <t>0.0152</t>
+  </si>
+  <si>
+    <t>8.4965</t>
   </si>
 </sst>
 </file>
@@ -112,13 +157,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -127,6 +169,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -444,83 +501,113 @@
   <dimension ref="C4:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="9" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="H4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>128</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>256</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>512</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1024</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>2048</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed tape algorithm memory leak
</commit_message>
<xml_diff>
--- a/lab6_cpp/Results.xlsx
+++ b/lab6_cpp/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tempRepo\sem5\DS\DS_labs3\lab6_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DC0E17-3A52-480A-9C41-6C198B0B522D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD7694B-F5EA-4E1F-ADE4-E66C6B9BFFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C4ADCE2E-1671-4732-8DDF-8B5F524DD51A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="41">
   <si>
     <t>Matrix Size</t>
   </si>
@@ -51,52 +51,112 @@
     <t>Serial Time</t>
   </si>
   <si>
-    <t>Fox</t>
-  </si>
-  <si>
     <t>0.0071</t>
   </si>
   <si>
-    <t>0.1292</t>
-  </si>
-  <si>
-    <t>1.2083</t>
-  </si>
-  <si>
-    <t>25.1591</t>
-  </si>
-  <si>
-    <t>242.1411</t>
-  </si>
-  <si>
-    <t>50.1231</t>
-  </si>
-  <si>
-    <t>4.8309</t>
-  </si>
-  <si>
-    <t>2.4463</t>
-  </si>
-  <si>
-    <t>10.2846</t>
-  </si>
-  <si>
-    <t>0.2472</t>
-  </si>
-  <si>
-    <t>4.8870</t>
-  </si>
-  <si>
     <t>0.0017</t>
   </si>
   <si>
-    <t>4.2527</t>
-  </si>
-  <si>
-    <t>0.0152</t>
-  </si>
-  <si>
-    <t>8.4965</t>
+    <t>Fox Algorithm (9 processors)</t>
+  </si>
+  <si>
+    <t>Cannon Algorithm (4 processors)</t>
+  </si>
+  <si>
+    <t>0.0023</t>
+  </si>
+  <si>
+    <t>0.0070</t>
+  </si>
+  <si>
+    <t>0.0902</t>
+  </si>
+  <si>
+    <t>0.7406</t>
+  </si>
+  <si>
+    <t>14.8260</t>
+  </si>
+  <si>
+    <t>168.0410</t>
+  </si>
+  <si>
+    <t>0.0255</t>
+  </si>
+  <si>
+    <t>0.2489</t>
+  </si>
+  <si>
+    <t>2.1788</t>
+  </si>
+  <si>
+    <t>49.1084</t>
+  </si>
+  <si>
+    <t>3.0823</t>
+  </si>
+  <si>
+    <t>3.5380</t>
+  </si>
+  <si>
+    <t>2.9755</t>
+  </si>
+  <si>
+    <t>6.8046</t>
+  </si>
+  <si>
+    <t>3.4218</t>
+  </si>
+  <si>
+    <t>Cannon Algorithm (9 processors)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tape Algorithm (9 processors)</t>
+  </si>
+  <si>
+    <t>Tape Algorithm (4 processors)</t>
+  </si>
+  <si>
+    <t>0.0218</t>
+  </si>
+  <si>
+    <t>0.2314</t>
+  </si>
+  <si>
+    <t>2.2117</t>
+  </si>
+  <si>
+    <t>47.9402</t>
+  </si>
+  <si>
+    <t>0.0890</t>
+  </si>
+  <si>
+    <t>0.7522</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14.3465</t>
+  </si>
+  <si>
+    <t>171.3783</t>
+  </si>
+  <si>
+    <t>4.1060</t>
+  </si>
+  <si>
+    <t>4.0856</t>
+  </si>
+  <si>
+    <t>3.2511</t>
+  </si>
+  <si>
+    <t>6.4867</t>
+  </si>
+  <si>
+    <t>3.5748</t>
   </si>
 </sst>
 </file>
@@ -122,12 +182,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -157,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -169,21 +235,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -498,36 +565,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB52D0A-4F56-4818-A1D0-703756E7ADF5}">
-  <dimension ref="C4:H10"/>
+  <dimension ref="C4:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="6" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="H4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="M4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -537,81 +621,477 @@
         <v>2</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="3">
         <v>128</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="3">
+        <v>128</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="3">
+        <v>128</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="4">
         <v>256</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="4">
+        <v>256</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M7" s="4">
+        <v>256</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="4">
         <v>512</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="D8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="4">
+        <v>512</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="K8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="4">
+        <v>512</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>1024</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1024</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1024</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="4">
         <v>2048</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>12</v>
+      <c r="D10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2048</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="4">
+        <v>2048</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="H19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="M19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>128</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="3">
+        <v>128</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="3">
+        <v>128</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="4">
+        <v>256</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="4">
+        <v>256</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="4">
+        <v>256</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="4">
+        <v>512</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="4">
+        <v>512</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="4">
+        <v>512</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
+        <v>1024</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1024</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1024</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>2048</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="4">
+        <v>2048</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="4">
+        <v>2048</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
     <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="M19:P19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
filled in results table
</commit_message>
<xml_diff>
--- a/lab6_cpp/Results.xlsx
+++ b/lab6_cpp/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tempRepo\sem5\DS\DS_labs3\lab6_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD7694B-F5EA-4E1F-ADE4-E66C6B9BFFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89216DA-FB87-45AF-8E34-CCA215345834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C4ADCE2E-1671-4732-8DDF-8B5F524DD51A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
   <si>
     <t>Matrix Size</t>
   </si>
@@ -157,6 +157,177 @@
   </si>
   <si>
     <t>3.5748</t>
+  </si>
+  <si>
+    <t>0.0133</t>
+  </si>
+  <si>
+    <t>0.1260</t>
+  </si>
+  <si>
+    <t>0.9517</t>
+  </si>
+  <si>
+    <t>7.7621</t>
+  </si>
+  <si>
+    <t>0.0059</t>
+  </si>
+  <si>
+    <t>0.0673</t>
+  </si>
+  <si>
+    <t>0.5770</t>
+  </si>
+  <si>
+    <t>11.3943</t>
+  </si>
+  <si>
+    <t>150.5690</t>
+  </si>
+  <si>
+    <t>3.3941</t>
+  </si>
+  <si>
+    <t>5.0667</t>
+  </si>
+  <si>
+    <t>4.5812</t>
+  </si>
+  <si>
+    <t>11.9721</t>
+  </si>
+  <si>
+    <t>19.3980</t>
+  </si>
+  <si>
+    <t>0.0015</t>
+  </si>
+  <si>
+    <t>0.0259</t>
+  </si>
+  <si>
+    <t>0.1764</t>
+  </si>
+  <si>
+    <t>0.7017</t>
+  </si>
+  <si>
+    <t>5.6313</t>
+  </si>
+  <si>
+    <t>0.0025</t>
+  </si>
+  <si>
+    <t>0.0791</t>
+  </si>
+  <si>
+    <t>0.6746</t>
+  </si>
+  <si>
+    <t>2.7733</t>
+  </si>
+  <si>
+    <t>18.1305</t>
+  </si>
+  <si>
+    <t>1.6885</t>
+  </si>
+  <si>
+    <t>3.0561</t>
+  </si>
+  <si>
+    <t>3.8235</t>
+  </si>
+  <si>
+    <t>3.9523</t>
+  </si>
+  <si>
+    <t>3.2196</t>
+  </si>
+  <si>
+    <t>0.2170</t>
+  </si>
+  <si>
+    <t>0.8815</t>
+  </si>
+  <si>
+    <t>0.0345</t>
+  </si>
+  <si>
+    <t>5.4933</t>
+  </si>
+  <si>
+    <t>0.0026</t>
+  </si>
+  <si>
+    <t>0.0796</t>
+  </si>
+  <si>
+    <t>0.6981</t>
+  </si>
+  <si>
+    <t>2.9752</t>
+  </si>
+  <si>
+    <t>17.8859</t>
+  </si>
+  <si>
+    <t>1.5307</t>
+  </si>
+  <si>
+    <t>2.3089</t>
+  </si>
+  <si>
+    <t>3.2179</t>
+  </si>
+  <si>
+    <t>3.3751</t>
+  </si>
+  <si>
+    <t>3.2559</t>
+  </si>
+  <si>
+    <t>11.0323</t>
+  </si>
+  <si>
+    <t>0.0013</t>
+  </si>
+  <si>
+    <t>0.0274</t>
+  </si>
+  <si>
+    <t>0.1708</t>
+  </si>
+  <si>
+    <t>0.5009</t>
+  </si>
+  <si>
+    <t>2.2901</t>
+  </si>
+  <si>
+    <t>0.0969</t>
+  </si>
+  <si>
+    <t>0.8964</t>
+  </si>
+  <si>
+    <t>3.4900</t>
+  </si>
+  <si>
+    <t>25.2653</t>
+  </si>
+  <si>
+    <t>2.0102</t>
+  </si>
+  <si>
+    <t>3.5356</t>
+  </si>
+  <si>
+    <t>5.2485</t>
+  </si>
+  <si>
+    <t>6.9678</t>
   </si>
 </sst>
 </file>
@@ -223,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -242,9 +413,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -568,7 +736,7 @@
   <dimension ref="C4:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,24 +756,24 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="H4" s="12" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="H4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="M4" s="10" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="M4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -650,7 +818,7 @@
       <c r="C6" s="3">
         <v>128</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -662,7 +830,7 @@
       <c r="H6" s="3">
         <v>128</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="7" t="s">
@@ -674,14 +842,14 @@
       <c r="M6" s="3">
         <v>128</v>
       </c>
-      <c r="N6" s="11" t="s">
-        <v>25</v>
+      <c r="N6" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
@@ -713,13 +881,13 @@
         <v>256</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
@@ -751,13 +919,13 @@
         <v>512</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
@@ -789,13 +957,13 @@
         <v>1024</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
@@ -827,34 +995,34 @@
         <v>2048</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="H19" s="10" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="H19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="M19" s="10" t="s">
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="M19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
@@ -896,192 +1064,192 @@
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="3">
-        <v>128</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="H21" s="3">
-        <v>128</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="M21" s="3">
-        <v>128</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="4">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="H22" s="4">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="M22" s="4">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="4">
-        <v>512</v>
+        <v>600</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="H23" s="4">
-        <v>512</v>
+        <v>600</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="M23" s="4">
-        <v>512</v>
+        <v>600</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="4">
-        <v>1024</v>
+        <v>900</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H24" s="4">
-        <v>1024</v>
+        <v>900</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="M24" s="4">
-        <v>1024</v>
+        <v>900</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="4">
-        <v>2048</v>
+        <v>1500</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="H25" s="4">
-        <v>2048</v>
+        <v>1500</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="M25" s="4">
-        <v>2048</v>
+        <v>1500</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>